<commit_message>
plots and idealisation fixed
Bugs in plotting and units fixed
Quadrilinear idealisation improved
Tested and compared with N2 method
</commit_message>
<xml_diff>
--- a/tests/NSP/fragility_process/test_simplified_method.xlsx
+++ b/tests/NSP/fragility_process/test_simplified_method.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="SINGLE-BUILDING" sheetId="1" r:id="rId1"/>
+    <sheet name="Foglio1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Tav</t>
   </si>
@@ -30,9 +31,6 @@
     <t>Sa_ratios</t>
   </si>
   <si>
-    <t>dy</t>
-  </si>
-  <si>
     <t>dcroof</t>
   </si>
   <si>
@@ -70,6 +68,12 @@
   </si>
   <si>
     <t>log_mean</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>SPO</t>
   </si>
 </sst>
 </file>
@@ -114,12 +118,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -131,7 +141,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -153,8 +163,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -162,8 +188,10 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="21">
+  <cellStyles count="37">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
@@ -174,6 +202,14 @@
     <cellStyle name="Collegamento ipertestuale" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento ipertestuale" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Collegamento ipertestuale" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
@@ -184,6 +220,14 @@
     <cellStyle name="Collegamento visitato" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Collegamento visitato" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Collegamento visitato" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -513,318 +557,270 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="2" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2">
-        <v>1.292</v>
+        <v>9.81</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>1.6120000000000001</v>
+        <v>1.1910000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4">
-        <f>AVERAGE(B3,C3,D3)</f>
-        <v>1.6120000000000001</v>
+        <v>1.081</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <f>AVERAGE(B4,C4,D4)</f>
+        <v>1.081</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>3.6765261666666667E-2</v>
-      </c>
-      <c r="C6">
-        <v>0.29044840199999999</v>
-      </c>
-      <c r="D6">
-        <v>2133.2600000000002</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:6">
       <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1">
-        <v>7.8100000000000003E-2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>0.1323</v>
-      </c>
-      <c r="D7" s="1">
-        <v>0.18690000000000001</v>
-      </c>
-      <c r="E7" s="1">
-        <v>0.24479999999999999</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0.29039999999999999</v>
+        <v>17</v>
+      </c>
+      <c r="B7">
+        <v>7.3672300529100496E-2</v>
+      </c>
+      <c r="C7">
+        <v>0.51132999999999895</v>
+      </c>
+      <c r="D7">
+        <v>251.88</v>
       </c>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>0</v>
-      </c>
-      <c r="C8">
-        <v>0</v>
-      </c>
-      <c r="D8">
-        <v>0.1</v>
-      </c>
-      <c r="E8">
-        <v>0.2</v>
-      </c>
-      <c r="F8">
-        <v>0.3</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9.5533999999999994E-2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.14565</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:6">
       <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9" s="5">
-        <f>B7/$B$6</f>
-        <v>2.124287886431925</v>
-      </c>
-      <c r="C9" s="5">
-        <f>C7/$B$6</f>
-        <v>3.59850560019134</v>
-      </c>
-      <c r="D9" s="5">
-        <f>D7/$B$6</f>
-        <v>5.0836031494766551</v>
-      </c>
-      <c r="E9" s="5">
-        <f>E7/$B$6</f>
-        <v>6.6584593418506426</v>
-      </c>
-      <c r="F9" s="5">
-        <f>F7/$B$6</f>
-        <v>7.8987605918032129</v>
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:6">
       <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="6">
-        <f>79.12*B3^1.98</f>
-        <v>203.64279672289135</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="B10" s="5">
+        <f>B8/$B$7</f>
+        <v>0.95015357871646844</v>
+      </c>
+      <c r="C10" s="5">
+        <f>C8/$B$7</f>
+        <v>1.2967424569871298</v>
+      </c>
+      <c r="D10" s="5">
+        <f>D8/$B$7</f>
+        <v>1.9769981248579087</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:6">
       <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" s="4">
-        <f>MAX(1.00001,0.425*(1-$B10+SQRT($B10^2+2*$B10*(2*B9-1)+1)))</f>
-        <v>1.7958319320318785</v>
-      </c>
-      <c r="C11" s="4">
-        <f t="shared" ref="C11:F11" si="0">MAX(1.00001,0.425*(1-$B10+SQRT($B10^2+2*$B10*(2*C9-1)+1)))</f>
-        <v>3.0208445988052604</v>
-      </c>
-      <c r="D11" s="4">
-        <f t="shared" si="0"/>
-        <v>4.2381079250319527</v>
-      </c>
-      <c r="E11" s="4">
-        <f t="shared" si="0"/>
-        <v>5.5112783104916137</v>
-      </c>
-      <c r="F11" s="4">
-        <f t="shared" si="0"/>
-        <v>6.5016646037909007</v>
+        <v>5</v>
+      </c>
+      <c r="B11" s="6">
+        <f>79.12*B4^1.98</f>
+        <v>92.31263602846397</v>
       </c>
     </row>
     <row r="12" spans="1:6">
       <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12" s="2">
-        <f>1+(B11-1)/$B10</f>
-        <v>1.0039079797804722</v>
-      </c>
-      <c r="C12" s="2">
-        <f t="shared" ref="C12:F12" si="1">1+(C11-1)/$B10</f>
-        <v>1.0099234769475061</v>
-      </c>
-      <c r="D12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0159009205193652</v>
-      </c>
-      <c r="E12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0221528990128257</v>
-      </c>
-      <c r="F12" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0270162494933583</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="B12" s="4">
+        <f>MAX(1.00001,0.425*(1-$B11+SQRT($B11^2+2*$B11*(2*B10-1)+1)))</f>
+        <v>1.0000100000000001</v>
+      </c>
+      <c r="C12" s="4">
+        <f t="shared" ref="C12:F12" si="0">MAX(1.00001,0.425*(1-$B11+SQRT($B11^2+2*$B11*(2*C10-1)+1)))</f>
+        <v>1.0987478965901645</v>
+      </c>
+      <c r="D12" s="4">
+        <f t="shared" si="0"/>
+        <v>1.663211053839041</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6">
       <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13" s="4">
-        <f>4*PI()^2/(9.81*$B2*B12*$B3^2)*B7</f>
-        <v>9.3251380163353895E-2</v>
-      </c>
-      <c r="C13" s="4">
-        <f>4*PI()^2/(9.81*$B2*C12*$B3^2)*C7</f>
-        <v>0.15702525844896112</v>
-      </c>
-      <c r="D13" s="4">
-        <f>4*PI()^2/(9.81*$B2*D12*$B3^2)*D7</f>
-        <v>0.22052411521174251</v>
-      </c>
-      <c r="E13" s="4">
-        <f>4*PI()^2/(9.81*$B2*E12*$B3^2)*E7</f>
-        <v>0.28707388685506746</v>
-      </c>
-      <c r="F13" s="4">
-        <f>4*PI()^2/(9.81*$B2*F12*$B3^2)*F7</f>
-        <v>0.33893579547023117</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="B13" s="2">
+        <f>1+(B12-1)/$B11</f>
+        <v>1.0000001083275316</v>
+      </c>
+      <c r="C13" s="2">
+        <f t="shared" ref="C13:F13" si="1">1+(C12-1)/$B11</f>
+        <v>1.00106971158921</v>
+      </c>
+      <c r="D13" s="2">
+        <f t="shared" si="1"/>
+        <v>1.0071844016417704</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6">
       <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <f>1+(LN(B12)/LN(B11))</f>
-        <v>1.0066619540084862</v>
-      </c>
-      <c r="C14" s="4">
-        <f t="shared" ref="C14:F14" si="2">1+(LN(C12)/LN(C11))</f>
-        <v>1.0089319194208031</v>
-      </c>
-      <c r="D14" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0109242021528921</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0128375509455829</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="2"/>
-        <v>1.0142398097376328</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="B14" s="7">
+        <f>4*PI()^2/(B2*$B3*B13*$B4^2)*B8</f>
+        <v>0.20240702094516769</v>
+      </c>
+      <c r="C14" s="7">
+        <f>4*PI()^2/(B2*$B3*C13*$B4^2)*C8</f>
+        <v>0.27594416837765862</v>
+      </c>
+      <c r="D14" s="7">
+        <f>4*PI()^2/(B2*$B3*D13*$B4^2)*D8</f>
+        <v>0.41814708899904263</v>
+      </c>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="3">
-        <f>1.957*(1/5.876+1/(($B3+0.1)*11.749))*(1-EXP(-0.739*(B11-1)))</f>
-        <v>0.19134350617986204</v>
-      </c>
-      <c r="C15" s="3">
-        <f t="shared" ref="C15:F15" si="3">1.957*(1/5.876+1/(($B3+0.1)*11.749))*(1-EXP(-0.739*(C11-1)))</f>
-        <v>0.33368561067790548</v>
-      </c>
-      <c r="D15" s="3">
-        <f t="shared" si="3"/>
-        <v>0.39102807395683359</v>
-      </c>
-      <c r="E15" s="3">
-        <f t="shared" si="3"/>
-        <v>0.41499933247059884</v>
-      </c>
-      <c r="F15" s="3">
-        <f t="shared" si="3"/>
-        <v>0.42296312296094896</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <f>1+(LN(B13)/LN(B12))</f>
+        <v>1.0108328067380197</v>
+      </c>
+      <c r="C15" s="4">
+        <f t="shared" ref="C15:F15" si="2">1+(LN(C13)/LN(C12))</f>
+        <v>1.0113531443123223</v>
+      </c>
+      <c r="D15" s="4">
+        <f t="shared" si="2"/>
+        <v>1.0140711848972426</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6">
       <c r="A16" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B16" s="3">
-        <f>SQRT(B15^2+B8^2)/B14</f>
-        <v>0.19007722047897024</v>
+        <f>1.957*(1/5.876+1/(($B4+0.1)*11.749))*(1-EXP(-0.739*(B12-1)))</f>
+        <v>3.5035044308044473E-6</v>
       </c>
       <c r="C16" s="3">
-        <f t="shared" ref="C16:F16" si="4">SQRT(C15^2+C8^2)/C14</f>
-        <v>0.33073154318426579</v>
+        <f t="shared" ref="C16:F16" si="3">1.957*(1/5.876+1/(($B4+0.1)*11.749))*(1-EXP(-0.739*(C12-1)))</f>
+        <v>3.3364316774056296E-2</v>
       </c>
       <c r="D16" s="3">
+        <f t="shared" si="3"/>
+        <v>0.18368235664563565</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="3">
+        <f>SQRT(B16^2+B9^2)/B15</f>
+        <v>3.4659583735814187E-6</v>
+      </c>
+      <c r="C17" s="3">
+        <f t="shared" ref="C17:F17" si="4">SQRT(C16^2+C9^2)/C15</f>
+        <v>3.298977905165127E-2</v>
+      </c>
+      <c r="D17" s="3">
         <f t="shared" si="4"/>
-        <v>0.39925088428187744</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="shared" si="4"/>
-        <v>0.45483922387190295</v>
-      </c>
-      <c r="F16" s="3">
-        <f t="shared" si="4"/>
-        <v>0.5112731362966545</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18">
-        <f>LN(B13)</f>
-        <v>-2.3724564198883429</v>
-      </c>
-      <c r="C18">
-        <f t="shared" ref="C18:F18" si="5">LN(C13)</f>
-        <v>-1.8513486047334078</v>
-      </c>
-      <c r="D18">
+        <v>0.18113359237620824</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="8">
+        <f>LN(B14)</f>
+        <v>-1.5974746537061901</v>
+      </c>
+      <c r="C19" s="8">
+        <f t="shared" ref="C19:F19" si="5">LN(C14)</f>
+        <v>-1.2875567222148068</v>
+      </c>
+      <c r="D19" s="8">
         <f t="shared" si="5"/>
-        <v>-1.511748224035617</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="5"/>
-        <v>-1.248015650867879</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="5"/>
-        <v>-1.0819445834320984</v>
-      </c>
+        <v>-0.8719220207977687</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="B24" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -835,4 +831,24 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B1" sqref="A1:XFD1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>